<commit_message>
Misc updates to different scripts
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Habitat_Quality_Restoration_and_Protection_Scoring.xlsx
+++ b/Data/Criteria_and_Scoring/Habitat_Quality_Restoration_and_Protection_Scoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF91912-D5C1-4356-84A8-158E5B668951}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D31FADD-1FC1-4701-AF11-38D51CB80938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1548" yWindow="1776" windowWidth="20196" windowHeight="10872" xr2:uid="{9D2762CD-0033-457E-BDB0-98D3A9FB6889}"/>
+    <workbookView xWindow="1656" yWindow="1248" windowWidth="20928" windowHeight="10668" xr2:uid="{9D2762CD-0033-457E-BDB0-98D3A9FB6889}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +485,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="C2" s="1">
         <v>0.8</v>
@@ -528,7 +528,7 @@
         <v>0.9</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -545,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="C5" s="1">
         <v>0.7</v>
@@ -588,7 +588,7 @@
         <v>0.9</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D7" s="2">
         <v>5</v>

</xml_diff>